<commit_message>
fixed flow chart bug - rework doc
</commit_message>
<xml_diff>
--- a/module/arduino/BigSwitch4Lamps/BigSwitchDesign.xlsx
+++ b/module/arduino/BigSwitch4Lamps/BigSwitchDesign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="22995" windowHeight="14055"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="22995" windowHeight="14055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="1" r:id="rId1"/>
@@ -91,10 +91,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -253,11 +266,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEA23C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBF6DD5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -331,9 +382,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +422,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -443,7 +494,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,11 +670,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="4.85546875" style="4" customWidth="1"/>
     <col min="4" max="9" width="9.140625" style="4"/>
@@ -663,13 +714,17 @@
         <v>0</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" t="s">
         <v>9</v>
@@ -685,10 +740,14 @@
       <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
@@ -696,9 +755,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="11">
+      <c r="F7" s="15">
         <v>1</v>
       </c>
       <c r="G7" s="11"/>
@@ -713,13 +774,15 @@
       <c r="C8" s="2"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="11"/>
-      <c r="G8" s="11">
-        <v>1</v>
-      </c>
-      <c r="H8" s="7"/>
+      <c r="G8" s="15">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -731,15 +794,19 @@
       <c r="D9" s="11">
         <v>1</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="15">
+        <v>0</v>
+      </c>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8"/>
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
@@ -747,7 +814,9 @@
         <v>5</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="15">
+        <v>0</v>
+      </c>
       <c r="E10" s="11">
         <v>1</v>
       </c>
@@ -755,9 +824,11 @@
         <v>1</v>
       </c>
       <c r="G10" s="11"/>
-      <c r="H10" s="7"/>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
       <c r="I10" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -766,14 +837,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="11">
-        <v>1</v>
-      </c>
+      <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="11">
-        <v>1</v>
-      </c>
+      <c r="G11" s="11"/>
       <c r="H11" s="7"/>
       <c r="I11" s="8"/>
     </row>
@@ -783,13 +850,9 @@
         <v>7</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="11">
-        <v>1</v>
-      </c>
+      <c r="D12" s="11"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="11">
-        <v>1</v>
-      </c>
+      <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
       <c r="I12" s="8"/>
@@ -801,13 +864,9 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="11">
-        <v>1</v>
-      </c>
+      <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="11">
-        <v>1</v>
-      </c>
+      <c r="G13" s="11"/>
       <c r="H13" s="7"/>
       <c r="I13" s="8"/>
     </row>
@@ -833,10 +892,16 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" t="s">
         <v>18</v>
@@ -848,10 +913,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="11">
+        <v>1</v>
+      </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="F16" s="15">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="8"/>
     </row>
@@ -861,12 +932,20 @@
         <v>2</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+      <c r="D17" s="15">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
+        <v>1</v>
+      </c>
       <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="G17" s="11">
+        <v>1</v>
+      </c>
       <c r="H17" s="7"/>
-      <c r="I17" s="8"/>
+      <c r="I17" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -874,9 +953,15 @@
         <v>3</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="D18" s="15">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11">
+        <v>1</v>
+      </c>
       <c r="G18" s="11"/>
       <c r="H18" s="7"/>
       <c r="I18" s="8"/>
@@ -887,12 +972,20 @@
         <v>4</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="D19" s="11">
+        <v>1</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
@@ -900,12 +993,22 @@
         <v>5</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="15">
+        <v>0</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="8"/>
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
@@ -968,10 +1071,16 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1</v>
+      </c>
       <c r="G25" s="11"/>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5">
+        <v>1</v>
+      </c>
       <c r="I25" s="6"/>
       <c r="J25" t="s">
         <v>17</v>
@@ -984,9 +1093,15 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="E26" s="11">
+        <v>1</v>
+      </c>
+      <c r="F26" s="15">
+        <v>0</v>
+      </c>
+      <c r="G26" s="11">
+        <v>1</v>
+      </c>
       <c r="H26" s="7"/>
       <c r="I26" s="8"/>
     </row>
@@ -996,11 +1111,17 @@
         <v>2</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="11"/>
+      <c r="D27" s="15">
+        <v>1</v>
+      </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="7"/>
+      <c r="G27" s="11">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7">
+        <v>1</v>
+      </c>
       <c r="I27" s="8"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1009,10 +1130,16 @@
         <v>3</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="11">
+        <v>1</v>
+      </c>
       <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="F28" s="11">
+        <v>1</v>
+      </c>
+      <c r="G28" s="15">
+        <v>0</v>
+      </c>
       <c r="H28" s="7"/>
       <c r="I28" s="8"/>
     </row>
@@ -1023,10 +1150,18 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="7"/>
+      <c r="E29" s="11">
+        <v>1</v>
+      </c>
+      <c r="F29" s="11">
+        <v>1</v>
+      </c>
+      <c r="G29" s="15">
+        <v>0</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1</v>
+      </c>
       <c r="I29" s="8"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1035,12 +1170,20 @@
         <v>5</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="D30" s="15">
+        <v>0</v>
+      </c>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
       <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="G30" s="11">
+        <v>1</v>
+      </c>
       <c r="H30" s="7"/>
-      <c r="I30" s="8"/>
+      <c r="I30" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
@@ -1048,12 +1191,22 @@
         <v>6</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="D31" s="15">
+        <v>0</v>
+      </c>
+      <c r="E31" s="11">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11">
+        <v>1</v>
+      </c>
       <c r="G31" s="11"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="8"/>
+      <c r="H31" s="7">
+        <v>0</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
@@ -1102,12 +1255,20 @@
         <v>0</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="D35" s="11">
+        <v>1</v>
+      </c>
+      <c r="E35" s="15">
+        <v>0</v>
+      </c>
+      <c r="F35" s="11">
+        <v>1</v>
+      </c>
       <c r="G35" s="11"/>
       <c r="H35" s="5"/>
-      <c r="I35" s="6"/>
+      <c r="I35" s="6">
+        <v>1</v>
+      </c>
       <c r="J35" t="s">
         <v>16</v>
       </c>
@@ -1119,10 +1280,18 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="7"/>
+      <c r="E36" s="11">
+        <v>1</v>
+      </c>
+      <c r="F36" s="11">
+        <v>1</v>
+      </c>
+      <c r="G36" s="15">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
+        <v>1</v>
+      </c>
       <c r="I36" s="8"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -1132,11 +1301,17 @@
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+      <c r="E37" s="11">
+        <v>1</v>
+      </c>
       <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="G37" s="15">
+        <v>1</v>
+      </c>
       <c r="H37" s="7"/>
-      <c r="I37" s="8"/>
+      <c r="I37" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
@@ -1144,11 +1319,19 @@
         <v>3</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="D38" s="11">
+        <v>1</v>
+      </c>
+      <c r="E38" s="15">
+        <v>0</v>
+      </c>
       <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="7"/>
+      <c r="G38" s="11">
+        <v>1</v>
+      </c>
+      <c r="H38" s="7">
+        <v>1</v>
+      </c>
       <c r="I38" s="8"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1157,9 +1340,13 @@
         <v>4</v>
       </c>
       <c r="C39" s="2"/>
-      <c r="D39" s="11"/>
+      <c r="D39" s="15">
+        <v>1</v>
+      </c>
       <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+      <c r="F39" s="11">
+        <v>1</v>
+      </c>
       <c r="G39" s="11"/>
       <c r="H39" s="7"/>
       <c r="I39" s="8"/>
@@ -1171,10 +1358,18 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="7"/>
+      <c r="E40" s="11">
+        <v>1</v>
+      </c>
+      <c r="F40" s="22">
+        <v>1</v>
+      </c>
+      <c r="G40" s="15">
+        <v>0</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1</v>
+      </c>
       <c r="I40" s="8"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -1183,12 +1378,20 @@
         <v>6</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
+      <c r="D41" s="15">
+        <v>0</v>
+      </c>
+      <c r="E41" s="11">
+        <v>1</v>
+      </c>
       <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="G41" s="11">
+        <v>1</v>
+      </c>
       <c r="H41" s="7"/>
-      <c r="I41" s="8"/>
+      <c r="I41" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
@@ -1196,12 +1399,22 @@
         <v>7</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
+      <c r="D42" s="15">
+        <v>0</v>
+      </c>
+      <c r="E42" s="11">
+        <v>1</v>
+      </c>
+      <c r="F42" s="11">
+        <v>1</v>
+      </c>
       <c r="G42" s="11"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="8"/>
+      <c r="H42" s="7">
+        <v>0</v>
+      </c>
+      <c r="I42" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
@@ -1238,10 +1451,16 @@
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="E45" s="15">
+        <v>1</v>
+      </c>
+      <c r="F45" s="11">
+        <v>1</v>
+      </c>
       <c r="G45" s="11"/>
-      <c r="H45" s="5"/>
+      <c r="H45" s="5">
+        <v>1</v>
+      </c>
       <c r="I45" s="6"/>
       <c r="J45" t="s">
         <v>15</v>
@@ -1254,9 +1473,15 @@
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
+      <c r="E46" s="11">
+        <v>1</v>
+      </c>
+      <c r="F46" s="15">
+        <v>0</v>
+      </c>
+      <c r="G46" s="11">
+        <v>1</v>
+      </c>
       <c r="H46" s="7"/>
       <c r="I46" s="8"/>
     </row>
@@ -1266,12 +1491,20 @@
         <v>2</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="D47" s="15">
+        <v>0</v>
+      </c>
+      <c r="E47" s="11">
+        <v>1</v>
+      </c>
+      <c r="F47" s="11">
+        <v>1</v>
+      </c>
       <c r="G47" s="11"/>
       <c r="H47" s="7"/>
-      <c r="I47" s="8"/>
+      <c r="I47" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
@@ -1279,11 +1512,17 @@
         <v>3</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="11"/>
+      <c r="D48" s="15">
+        <v>1</v>
+      </c>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="F48" s="11">
+        <v>1</v>
+      </c>
       <c r="G48" s="11"/>
-      <c r="H48" s="7"/>
+      <c r="H48" s="7">
+        <v>1</v>
+      </c>
       <c r="I48" s="8"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -1293,9 +1532,15 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
+      <c r="E49" s="11">
+        <v>1</v>
+      </c>
+      <c r="F49" s="11">
+        <v>1</v>
+      </c>
+      <c r="G49" s="15">
+        <v>0</v>
+      </c>
       <c r="H49" s="7"/>
       <c r="I49" s="8"/>
     </row>
@@ -1305,12 +1550,20 @@
         <v>5</v>
       </c>
       <c r="C50" s="2"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="D50" s="11">
+        <v>1</v>
+      </c>
+      <c r="E50" s="15">
+        <v>0</v>
+      </c>
+      <c r="F50" s="11">
+        <v>1</v>
+      </c>
       <c r="G50" s="11"/>
       <c r="H50" s="7"/>
-      <c r="I50" s="8"/>
+      <c r="I50" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
@@ -1318,12 +1571,22 @@
         <v>6</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="D51" s="15">
+        <v>0</v>
+      </c>
+      <c r="E51" s="11">
+        <v>1</v>
+      </c>
+      <c r="F51" s="11">
+        <v>1</v>
+      </c>
       <c r="G51" s="11"/>
-      <c r="H51" s="7"/>
-      <c r="I51" s="8"/>
+      <c r="H51" s="7">
+        <v>0</v>
+      </c>
+      <c r="I51" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
@@ -1373,10 +1636,16 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+      <c r="E55" s="15">
+        <v>1</v>
+      </c>
       <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="5"/>
+      <c r="G55" s="11">
+        <v>1</v>
+      </c>
+      <c r="H55" s="5">
+        <v>1</v>
+      </c>
       <c r="I55" s="6"/>
       <c r="J55" t="s">
         <v>14</v>
@@ -1389,11 +1658,17 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
+      <c r="E56" s="11">
+        <v>1</v>
+      </c>
+      <c r="F56" s="15">
+        <v>1</v>
+      </c>
       <c r="G56" s="11"/>
       <c r="H56" s="7"/>
-      <c r="I56" s="8"/>
+      <c r="I56" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
@@ -1402,10 +1677,18 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="7"/>
+      <c r="E57" s="11">
+        <v>1</v>
+      </c>
+      <c r="F57" s="15">
+        <v>0</v>
+      </c>
+      <c r="G57" s="11">
+        <v>1</v>
+      </c>
+      <c r="H57" s="7">
+        <v>1</v>
+      </c>
       <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -1414,10 +1697,14 @@
         <v>3</v>
       </c>
       <c r="C58" s="2"/>
-      <c r="D58" s="11"/>
+      <c r="D58" s="15">
+        <v>1</v>
+      </c>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
+      <c r="G58" s="11">
+        <v>1</v>
+      </c>
       <c r="H58" s="7"/>
       <c r="I58" s="8"/>
     </row>
@@ -1427,11 +1714,19 @@
         <v>4</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" s="11"/>
+      <c r="D59" s="11">
+        <v>1</v>
+      </c>
       <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="7"/>
+      <c r="F59" s="11">
+        <v>1</v>
+      </c>
+      <c r="G59" s="15">
+        <v>0</v>
+      </c>
+      <c r="H59" s="7">
+        <v>1</v>
+      </c>
       <c r="I59" s="8"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -1440,12 +1735,20 @@
         <v>5</v>
       </c>
       <c r="C60" s="2"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="D60" s="15">
+        <v>0</v>
+      </c>
+      <c r="E60" s="11">
+        <v>1</v>
+      </c>
+      <c r="F60" s="11">
+        <v>1</v>
+      </c>
       <c r="G60" s="11"/>
       <c r="H60" s="7"/>
-      <c r="I60" s="8"/>
+      <c r="I60" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
@@ -1453,12 +1756,22 @@
         <v>6</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
+      <c r="D61" s="15">
+        <v>0</v>
+      </c>
+      <c r="E61" s="11">
+        <v>1</v>
+      </c>
       <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="8"/>
+      <c r="G61" s="11">
+        <v>1</v>
+      </c>
+      <c r="H61" s="7">
+        <v>0</v>
+      </c>
+      <c r="I61" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
@@ -1507,12 +1820,20 @@
         <v>0</v>
       </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
+      <c r="D65" s="11">
+        <v>1</v>
+      </c>
+      <c r="E65" s="15">
+        <v>0</v>
+      </c>
       <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
+      <c r="G65" s="11">
+        <v>1</v>
+      </c>
       <c r="H65" s="5"/>
-      <c r="I65" s="6"/>
+      <c r="I65" s="6">
+        <v>1</v>
+      </c>
       <c r="J65" t="s">
         <v>13</v>
       </c>
@@ -1524,9 +1845,13 @@
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
+      <c r="E66" s="11">
+        <v>1</v>
+      </c>
       <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
+      <c r="G66" s="15">
+        <v>1</v>
+      </c>
       <c r="H66" s="7"/>
       <c r="I66" s="8"/>
     </row>
@@ -1537,11 +1862,19 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
+      <c r="E67" s="11">
+        <v>1</v>
+      </c>
+      <c r="F67" s="11">
+        <v>1</v>
+      </c>
+      <c r="G67" s="15">
+        <v>0</v>
+      </c>
       <c r="H67" s="7"/>
-      <c r="I67" s="8"/>
+      <c r="I67" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
@@ -1550,10 +1883,18 @@
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="7"/>
+      <c r="E68" s="11">
+        <v>1</v>
+      </c>
+      <c r="F68" s="15">
+        <v>0</v>
+      </c>
+      <c r="G68" s="11">
+        <v>1</v>
+      </c>
+      <c r="H68" s="7">
+        <v>1</v>
+      </c>
       <c r="I68" s="8"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -1563,9 +1904,15 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
+      <c r="E69" s="11">
+        <v>1</v>
+      </c>
+      <c r="F69" s="11">
+        <v>1</v>
+      </c>
+      <c r="G69" s="15">
+        <v>0</v>
+      </c>
       <c r="H69" s="7"/>
       <c r="I69" s="8"/>
     </row>
@@ -1575,12 +1922,20 @@
         <v>5</v>
       </c>
       <c r="C70" s="2"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
+      <c r="D70" s="11">
+        <v>1</v>
+      </c>
+      <c r="E70" s="15">
+        <v>0</v>
+      </c>
+      <c r="F70" s="11">
+        <v>1</v>
+      </c>
       <c r="G70" s="11"/>
       <c r="H70" s="7"/>
-      <c r="I70" s="8"/>
+      <c r="I70" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
@@ -1588,12 +1943,22 @@
         <v>6</v>
       </c>
       <c r="C71" s="2"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+      <c r="D71" s="15">
+        <v>0</v>
+      </c>
+      <c r="E71" s="11">
+        <v>1</v>
+      </c>
+      <c r="F71" s="11">
+        <v>1</v>
+      </c>
       <c r="G71" s="11"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="8"/>
+      <c r="H71" s="7">
+        <v>0</v>
+      </c>
+      <c r="I71" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
@@ -1642,12 +2007,20 @@
         <v>0</v>
       </c>
       <c r="C75" s="1"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="D75" s="11">
+        <v>1</v>
+      </c>
+      <c r="E75" s="15">
+        <v>0</v>
+      </c>
       <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
+      <c r="G75" s="11">
+        <v>1</v>
+      </c>
       <c r="H75" s="5"/>
-      <c r="I75" s="6"/>
+      <c r="I75" s="6">
+        <v>1</v>
+      </c>
       <c r="J75" t="s">
         <v>12</v>
       </c>
@@ -1658,11 +2031,19 @@
         <v>1</v>
       </c>
       <c r="C76" s="2"/>
-      <c r="D76" s="11"/>
+      <c r="D76" s="11">
+        <v>1</v>
+      </c>
       <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="7"/>
+      <c r="F76" s="11">
+        <v>1</v>
+      </c>
+      <c r="G76" s="15">
+        <v>0</v>
+      </c>
+      <c r="H76" s="7">
+        <v>1</v>
+      </c>
       <c r="I76" s="8"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -1671,12 +2052,18 @@
         <v>2</v>
       </c>
       <c r="C77" s="2"/>
-      <c r="D77" s="11"/>
+      <c r="D77" s="11">
+        <v>1</v>
+      </c>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
+      <c r="G77" s="15">
+        <v>1</v>
+      </c>
       <c r="H77" s="7"/>
-      <c r="I77" s="8"/>
+      <c r="I77" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
@@ -1685,9 +2072,13 @@
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
+      <c r="E78" s="15">
+        <v>1</v>
+      </c>
       <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
+      <c r="G78" s="11">
+        <v>1</v>
+      </c>
       <c r="H78" s="7"/>
       <c r="I78" s="8"/>
     </row>
@@ -1698,11 +2089,19 @@
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
+      <c r="E79" s="11">
+        <v>1</v>
+      </c>
+      <c r="F79" s="11">
+        <v>1</v>
+      </c>
+      <c r="G79" s="15">
+        <v>0</v>
+      </c>
       <c r="H79" s="7"/>
-      <c r="I79" s="8"/>
+      <c r="I79" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
@@ -1710,9 +2109,13 @@
         <v>5</v>
       </c>
       <c r="C80" s="2"/>
-      <c r="D80" s="11"/>
+      <c r="D80" s="11">
+        <v>1</v>
+      </c>
       <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="F80" s="15">
+        <v>1</v>
+      </c>
       <c r="G80" s="11"/>
       <c r="H80" s="7"/>
       <c r="I80" s="8"/>
@@ -1723,11 +2126,17 @@
         <v>6</v>
       </c>
       <c r="C81" s="2"/>
-      <c r="D81" s="11"/>
+      <c r="D81" s="11">
+        <v>1</v>
+      </c>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="7"/>
+      <c r="G81" s="15">
+        <v>1</v>
+      </c>
+      <c r="H81" s="7">
+        <v>1</v>
+      </c>
       <c r="I81" s="8"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -1736,12 +2145,20 @@
         <v>7</v>
       </c>
       <c r="C82" s="2"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
+      <c r="D82" s="11">
+        <v>1</v>
+      </c>
+      <c r="E82" s="15">
+        <v>0</v>
+      </c>
+      <c r="F82" s="11">
+        <v>1</v>
+      </c>
       <c r="G82" s="11"/>
       <c r="H82" s="7"/>
-      <c r="I82" s="8"/>
+      <c r="I82" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
@@ -1749,12 +2166,22 @@
         <v>8</v>
       </c>
       <c r="C83" s="2"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
+      <c r="D83" s="15">
+        <v>0</v>
+      </c>
+      <c r="E83" s="11">
+        <v>1</v>
+      </c>
+      <c r="F83" s="11">
+        <v>1</v>
+      </c>
       <c r="G83" s="11"/>
-      <c r="H83" s="7"/>
-      <c r="I83" s="8"/>
+      <c r="H83" s="7">
+        <v>0</v>
+      </c>
+      <c r="I83" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="14"/>
@@ -1777,12 +2204,20 @@
         <v>0</v>
       </c>
       <c r="C85" s="1"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
+      <c r="D85" s="11">
+        <v>1</v>
+      </c>
+      <c r="E85" s="15">
+        <v>0</v>
+      </c>
+      <c r="F85" s="11">
+        <v>1</v>
+      </c>
       <c r="G85" s="11"/>
       <c r="H85" s="5"/>
-      <c r="I85" s="6"/>
+      <c r="I85" s="6">
+        <v>1</v>
+      </c>
       <c r="J85" t="s">
         <v>11</v>
       </c>
@@ -1794,10 +2229,18 @@
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="7"/>
+      <c r="E86" s="11">
+        <v>1</v>
+      </c>
+      <c r="F86" s="11">
+        <v>1</v>
+      </c>
+      <c r="G86" s="15">
+        <v>0</v>
+      </c>
+      <c r="H86" s="7">
+        <v>1</v>
+      </c>
       <c r="I86" s="8"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -1807,11 +2250,17 @@
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
+      <c r="E87" s="11">
+        <v>1</v>
+      </c>
       <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
+      <c r="G87" s="15">
+        <v>1</v>
+      </c>
       <c r="H87" s="7"/>
-      <c r="I87" s="8"/>
+      <c r="I87" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
@@ -1819,11 +2268,19 @@
         <v>3</v>
       </c>
       <c r="C88" s="2"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
+      <c r="D88" s="11">
+        <v>1</v>
+      </c>
+      <c r="E88" s="15">
+        <v>0</v>
+      </c>
       <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="7"/>
+      <c r="G88" s="11">
+        <v>1</v>
+      </c>
+      <c r="H88" s="7">
+        <v>1</v>
+      </c>
       <c r="I88" s="8"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -1832,9 +2289,13 @@
         <v>4</v>
       </c>
       <c r="C89" s="2"/>
-      <c r="D89" s="11"/>
+      <c r="D89" s="15">
+        <v>1</v>
+      </c>
       <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
+      <c r="F89" s="11">
+        <v>1</v>
+      </c>
       <c r="G89" s="11"/>
       <c r="H89" s="7"/>
       <c r="I89" s="8"/>
@@ -1846,11 +2307,17 @@
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
+      <c r="E90" s="11">
+        <v>1</v>
+      </c>
       <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
+      <c r="G90" s="15">
+        <v>1</v>
+      </c>
       <c r="H90" s="7"/>
-      <c r="I90" s="8"/>
+      <c r="I90" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
@@ -1858,9 +2325,15 @@
         <v>6</v>
       </c>
       <c r="C91" s="2"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
+      <c r="D91" s="15">
+        <v>0</v>
+      </c>
+      <c r="E91" s="11">
+        <v>1</v>
+      </c>
+      <c r="F91" s="11">
+        <v>1</v>
+      </c>
       <c r="G91" s="11"/>
       <c r="H91" s="7"/>
       <c r="I91" s="8"/>
@@ -1871,12 +2344,20 @@
         <v>7</v>
       </c>
       <c r="C92" s="2"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
+      <c r="D92" s="11">
+        <v>1</v>
+      </c>
+      <c r="E92" s="15">
+        <v>0</v>
+      </c>
       <c r="F92" s="11"/>
-      <c r="G92" s="11"/>
+      <c r="G92" s="11">
+        <v>1</v>
+      </c>
       <c r="H92" s="7"/>
-      <c r="I92" s="8"/>
+      <c r="I92" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
@@ -1884,12 +2365,22 @@
         <v>8</v>
       </c>
       <c r="C93" s="2"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
+      <c r="D93" s="15">
+        <v>0</v>
+      </c>
+      <c r="E93" s="11">
+        <v>1</v>
+      </c>
       <c r="F93" s="11"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="8"/>
+      <c r="G93" s="11">
+        <v>1</v>
+      </c>
+      <c r="H93" s="7">
+        <v>0</v>
+      </c>
+      <c r="I93" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="14"/>
@@ -1912,12 +2403,20 @@
         <v>0</v>
       </c>
       <c r="C95" s="1"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
+      <c r="D95" s="11">
+        <v>1</v>
+      </c>
+      <c r="E95" s="15">
+        <v>0</v>
+      </c>
       <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="5"/>
-      <c r="I95" s="6"/>
+      <c r="G95" s="11">
+        <v>1</v>
+      </c>
+      <c r="H95" s="16"/>
+      <c r="I95" s="17">
+        <v>1</v>
+      </c>
       <c r="J95" t="s">
         <v>10</v>
       </c>
@@ -1928,12 +2427,20 @@
         <v>1</v>
       </c>
       <c r="C96" s="2"/>
-      <c r="D96" s="11"/>
+      <c r="D96" s="11">
+        <v>1</v>
+      </c>
       <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="7"/>
-      <c r="I96" s="8"/>
+      <c r="F96" s="11">
+        <v>1</v>
+      </c>
+      <c r="G96" s="15">
+        <v>0</v>
+      </c>
+      <c r="H96" s="18">
+        <v>1</v>
+      </c>
+      <c r="I96" s="19"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
@@ -1941,12 +2448,18 @@
         <v>2</v>
       </c>
       <c r="C97" s="2"/>
-      <c r="D97" s="11"/>
+      <c r="D97" s="11">
+        <v>1</v>
+      </c>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="7"/>
-      <c r="I97" s="8"/>
+      <c r="G97" s="15">
+        <v>1</v>
+      </c>
+      <c r="H97" s="18"/>
+      <c r="I97" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
@@ -1954,12 +2467,20 @@
         <v>3</v>
       </c>
       <c r="C98" s="2"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
+      <c r="D98" s="11">
+        <v>1</v>
+      </c>
+      <c r="E98" s="15">
+        <v>0</v>
+      </c>
+      <c r="F98" s="11">
+        <v>1</v>
+      </c>
       <c r="G98" s="11"/>
-      <c r="H98" s="7"/>
-      <c r="I98" s="8"/>
+      <c r="H98" s="18">
+        <v>1</v>
+      </c>
+      <c r="I98" s="19"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
@@ -1967,12 +2488,20 @@
         <v>4</v>
       </c>
       <c r="C99" s="2"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
+      <c r="D99" s="15">
+        <v>0</v>
+      </c>
+      <c r="E99" s="11">
+        <v>1</v>
+      </c>
       <c r="F99" s="11"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="7"/>
-      <c r="I99" s="8"/>
+      <c r="G99" s="11">
+        <v>1</v>
+      </c>
+      <c r="H99" s="18"/>
+      <c r="I99" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
@@ -1980,12 +2509,20 @@
         <v>5</v>
       </c>
       <c r="C100" s="2"/>
-      <c r="D100" s="11"/>
+      <c r="D100" s="11">
+        <v>1</v>
+      </c>
       <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="7"/>
-      <c r="I100" s="8"/>
+      <c r="F100" s="15">
+        <v>0</v>
+      </c>
+      <c r="G100" s="11">
+        <v>1</v>
+      </c>
+      <c r="H100" s="18">
+        <v>1</v>
+      </c>
+      <c r="I100" s="19"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
@@ -1993,12 +2530,18 @@
         <v>6</v>
       </c>
       <c r="C101" s="2"/>
-      <c r="D101" s="11"/>
+      <c r="D101" s="11">
+        <v>1</v>
+      </c>
       <c r="E101" s="11"/>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="7"/>
-      <c r="I101" s="8"/>
+      <c r="F101" s="11">
+        <v>1</v>
+      </c>
+      <c r="G101" s="15">
+        <v>0</v>
+      </c>
+      <c r="H101" s="18"/>
+      <c r="I101" s="19"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13"/>
@@ -2006,12 +2549,20 @@
         <v>7</v>
       </c>
       <c r="C102" s="2"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
+      <c r="D102" s="11">
+        <v>1</v>
+      </c>
+      <c r="E102" s="15">
+        <v>0</v>
+      </c>
       <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="7"/>
-      <c r="I102" s="8"/>
+      <c r="G102" s="11">
+        <v>1</v>
+      </c>
+      <c r="H102" s="18"/>
+      <c r="I102" s="19">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
@@ -2019,12 +2570,22 @@
         <v>8</v>
       </c>
       <c r="C103" s="2"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
+      <c r="D103" s="15">
+        <v>0</v>
+      </c>
+      <c r="E103" s="11">
+        <v>1</v>
+      </c>
+      <c r="F103" s="11">
+        <v>1</v>
+      </c>
       <c r="G103" s="11"/>
-      <c r="H103" s="7"/>
-      <c r="I103" s="8"/>
+      <c r="H103" s="18">
+        <v>0</v>
+      </c>
+      <c r="I103" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
@@ -2036,46 +2597,56 @@
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
       <c r="G104" s="11"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="10"/>
+      <c r="H104" s="20"/>
+      <c r="I104" s="21"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D5">
+  <conditionalFormatting sqref="D5:D36 D38:D44 F6:F36 F38:F44">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E36 E38:E44 G6:G36 G38:G44">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="G5">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
+  <conditionalFormatting sqref="D45:D104">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="F45:F104">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:D104">
+  <conditionalFormatting sqref="E45:E104">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:F104">
+  <conditionalFormatting sqref="G45:G104">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6:E104">
+  <conditionalFormatting sqref="D37 F37">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G104">
+  <conditionalFormatting sqref="E37 G37">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2089,11 +2660,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="1.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="1.5703125" bestFit="1" customWidth="1"/>
@@ -2117,14 +2688,14 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>Design!D5+2*Design!E5+4*Design!F5+8*Design!G5</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
         <f>Design!H5+2*Design!I5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -2136,14 +2707,14 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>Design!D6+2*Design!E6+4*Design!F6+8*Design!G6</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6">
         <f>Design!H6+2*Design!I6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -2152,7 +2723,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>Design!D7+2*Design!E7+4*Design!F7+8*Design!G7</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -2168,14 +2739,14 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>Design!D8+2*Design!E8+4*Design!F8+8*Design!G8</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
         <f>Design!H8+2*Design!I8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -2184,14 +2755,14 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>Design!D9+2*Design!E9+4*Design!F9+8*Design!G9</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9">
         <f>Design!H9+2*Design!I9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -2207,7 +2778,7 @@
       </c>
       <c r="C10">
         <f>Design!H10+2*Design!I10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -2216,7 +2787,7 @@
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>Design!D11+2*Design!E11+4*Design!F11+8*Design!G11</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -2232,7 +2803,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>Design!D12+2*Design!E12+4*Design!F12+8*Design!G12</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -2248,7 +2819,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>Design!D13+2*Design!E13+4*Design!F13+8*Design!G13</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -2280,14 +2851,14 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>Design!D15+2*Design!E15+4*Design!F15+8*Design!G15</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15">
         <f>Design!H15+2*Design!I15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
@@ -2299,7 +2870,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>Design!D16+2*Design!E16+4*Design!F16+8*Design!G16</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -2315,14 +2886,14 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>Design!D17+2*Design!E17+4*Design!F17+8*Design!G17</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17">
         <f>Design!H17+2*Design!I17</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
@@ -2331,7 +2902,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>Design!D18+2*Design!E18+4*Design!F18+8*Design!G18</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -2347,14 +2918,14 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>Design!D19+2*Design!E19+4*Design!F19+8*Design!G19</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19">
         <f>Design!H19+2*Design!I19</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
@@ -2363,7 +2934,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>Design!D20+2*Design!E20+4*Design!F20+8*Design!G20</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -2443,14 +3014,14 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>Design!D25+2*Design!E25+4*Design!F25+8*Design!G25</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25">
         <f>Design!H25+2*Design!I25</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
@@ -2462,7 +3033,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>Design!D26+2*Design!E26+4*Design!F26+8*Design!G26</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -2478,14 +3049,14 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>Design!D27+2*Design!E27+4*Design!F27+8*Design!G27</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27">
         <f>Design!H27+2*Design!I27</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
@@ -2494,7 +3065,7 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>Design!D28+2*Design!E28+4*Design!F28+8*Design!G28</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -2510,14 +3081,14 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>Design!D29+2*Design!E29+4*Design!F29+8*Design!G29</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29">
         <f>Design!H29+2*Design!I29</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -2526,14 +3097,14 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>Design!D30+2*Design!E30+4*Design!F30+8*Design!G30</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30">
         <f>Design!H30+2*Design!I30</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -2542,7 +3113,7 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>Design!D31+2*Design!E31+4*Design!F31+8*Design!G31</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -2606,14 +3177,14 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>Design!D35+2*Design!E35+4*Design!F35+8*Design!G35</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35">
         <f>Design!H35+2*Design!I35</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
@@ -2625,14 +3196,14 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>Design!D36+2*Design!E36+4*Design!F36+8*Design!G36</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36">
         <f>Design!H36+2*Design!I36</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
@@ -2640,15 +3211,15 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>Design!D37+2*Design!E37+4*Design!F37+8*Design!G37</f>
-        <v>0</v>
+        <f>Design!D38+2*Design!E38+4*Design!F38+8*Design!G38</f>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37">
         <f>Design!H37+2*Design!I37</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
@@ -2656,15 +3227,15 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>Design!D38+2*Design!E38+4*Design!F38+8*Design!G38</f>
-        <v>0</v>
+        <f>Design!D39+2*Design!E39+4*Design!F39+8*Design!G39</f>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38">
         <f>Design!H38+2*Design!I38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
@@ -2672,8 +3243,8 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>Design!D39+2*Design!E39+4*Design!F39+8*Design!G39</f>
-        <v>0</v>
+        <f>Design!D40+2*Design!E40+4*Design!F40+8*Design!G40</f>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -2688,15 +3259,15 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>Design!D40+2*Design!E40+4*Design!F40+8*Design!G40</f>
-        <v>0</v>
+        <f>Design!D41+2*Design!E41+4*Design!F41+8*Design!G41</f>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40">
         <f>Design!H40+2*Design!I40</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
         <v>8</v>
@@ -2704,15 +3275,15 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>Design!D41+2*Design!E41+4*Design!F41+8*Design!G41</f>
-        <v>0</v>
+        <f>Design!D42+2*Design!E42+4*Design!F42+8*Design!G42</f>
+        <v>6</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
       <c r="C41">
         <f>Design!H41+2*Design!I41</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
@@ -2720,7 +3291,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>Design!D42+2*Design!E42+4*Design!F42+8*Design!G42</f>
+        <f>Design!D43+2*Design!E43+4*Design!F43+8*Design!G43</f>
         <v>0</v>
       </c>
       <c r="B42" t="s">
@@ -2736,7 +3307,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>Design!D43+2*Design!E43+4*Design!F43+8*Design!G43</f>
+        <f>Design!D44+2*Design!E44+4*Design!F44+8*Design!G44</f>
         <v>0</v>
       </c>
       <c r="B43" t="s">
@@ -2751,9 +3322,9 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <f>Design!D44+2*Design!E44+4*Design!F44+8*Design!G44</f>
-        <v>0</v>
+      <c r="A44" t="e">
+        <f>Design!#REF!+2*Design!#REF!+4*Design!#REF!+8*Design!#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -2769,14 +3340,14 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>Design!D45+2*Design!E45+4*Design!F45+8*Design!G45</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45">
         <f>Design!H45+2*Design!I45</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
@@ -2788,7 +3359,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>Design!D46+2*Design!E46+4*Design!F46+8*Design!G46</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -2804,14 +3375,14 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>Design!D47+2*Design!E47+4*Design!F47+8*Design!G47</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
       </c>
       <c r="C47">
         <f>Design!H47+2*Design!I47</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
         <v>8</v>
@@ -2820,14 +3391,14 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>Design!D48+2*Design!E48+4*Design!F48+8*Design!G48</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
       </c>
       <c r="C48">
         <f>Design!H48+2*Design!I48</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="s">
         <v>8</v>
@@ -2836,7 +3407,7 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>Design!D49+2*Design!E49+4*Design!F49+8*Design!G49</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
@@ -2852,14 +3423,14 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>Design!D50+2*Design!E50+4*Design!F50+8*Design!G50</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
       <c r="C50">
         <f>Design!H50+2*Design!I50</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
@@ -2868,7 +3439,7 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>Design!D51+2*Design!E51+4*Design!F51+8*Design!G51</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
@@ -2932,14 +3503,14 @@
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>Design!D55+2*Design!E55+4*Design!F55+8*Design!G55</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55">
         <f>Design!H55+2*Design!I55</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" t="s">
         <v>8</v>
@@ -2951,14 +3522,14 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>Design!D56+2*Design!E56+4*Design!F56+8*Design!G56</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
       </c>
       <c r="C56">
         <f>Design!H56+2*Design!I56</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
@@ -2967,14 +3538,14 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <f>Design!D57+2*Design!E57+4*Design!F57+8*Design!G57</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
       </c>
       <c r="C57">
         <f>Design!H57+2*Design!I57</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
@@ -2983,7 +3554,7 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <f>Design!D58+2*Design!E58+4*Design!F58+8*Design!G58</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -2999,14 +3570,14 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <f>Design!D59+2*Design!E59+4*Design!F59+8*Design!G59</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
       </c>
       <c r="C59">
         <f>Design!H59+2*Design!I59</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" t="s">
         <v>8</v>
@@ -3015,14 +3586,14 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <f>Design!D60+2*Design!E60+4*Design!F60+8*Design!G60</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
       </c>
       <c r="C60">
         <f>Design!H60+2*Design!I60</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
         <v>8</v>
@@ -3031,7 +3602,7 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <f>Design!D61+2*Design!E61+4*Design!F61+8*Design!G61</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -3095,14 +3666,14 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <f>Design!D65+2*Design!E65+4*Design!F65+8*Design!G65</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65">
         <f>Design!H65+2*Design!I65</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D65" t="s">
         <v>8</v>
@@ -3114,7 +3685,7 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <f>Design!D66+2*Design!E66+4*Design!F66+8*Design!G66</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
@@ -3130,14 +3701,14 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <f>Design!D67+2*Design!E67+4*Design!F67+8*Design!G67</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
       </c>
       <c r="C67">
         <f>Design!H67+2*Design!I67</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D67" t="s">
         <v>8</v>
@@ -3146,14 +3717,14 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <f>Design!D68+2*Design!E68+4*Design!F68+8*Design!G68</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
       </c>
       <c r="C68">
         <f>Design!H68+2*Design!I68</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" t="s">
         <v>8</v>
@@ -3162,7 +3733,7 @@
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>Design!D69+2*Design!E69+4*Design!F69+8*Design!G69</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
@@ -3178,14 +3749,14 @@
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <f>Design!D70+2*Design!E70+4*Design!F70+8*Design!G70</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
       </c>
       <c r="C70">
         <f>Design!H70+2*Design!I70</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
@@ -3194,7 +3765,7 @@
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>Design!D71+2*Design!E71+4*Design!F71+8*Design!G71</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -3258,14 +3829,14 @@
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <f>Design!D75+2*Design!E75+4*Design!F75+8*Design!G75</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
       </c>
       <c r="C75">
         <f>Design!H75+2*Design!I75</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
         <v>8</v>
@@ -3277,14 +3848,14 @@
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <f>Design!D76+2*Design!E76+4*Design!F76+8*Design!G76</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
         <v>8</v>
       </c>
       <c r="C76">
         <f>Design!H76+2*Design!I76</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" t="s">
         <v>8</v>
@@ -3293,14 +3864,14 @@
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <f>Design!D77+2*Design!E77+4*Design!F77+8*Design!G77</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
         <v>8</v>
       </c>
       <c r="C77">
         <f>Design!H77+2*Design!I77</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
         <v>8</v>
@@ -3309,7 +3880,7 @@
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <f>Design!D78+2*Design!E78+4*Design!F78+8*Design!G78</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B78" t="s">
         <v>8</v>
@@ -3325,14 +3896,14 @@
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <f>Design!D79+2*Design!E79+4*Design!F79+8*Design!G79</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
       </c>
       <c r="C79">
         <f>Design!H79+2*Design!I79</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79" t="s">
         <v>8</v>
@@ -3341,7 +3912,7 @@
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <f>Design!D80+2*Design!E80+4*Design!F80+8*Design!G80</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
@@ -3357,14 +3928,14 @@
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <f>Design!D81+2*Design!E81+4*Design!F81+8*Design!G81</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
       </c>
       <c r="C81">
         <f>Design!H81+2*Design!I81</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
         <v>8</v>
@@ -3373,14 +3944,14 @@
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <f>Design!D82+2*Design!E82+4*Design!F82+8*Design!G82</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
       </c>
       <c r="C82">
         <f>Design!H82+2*Design!I82</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D82" t="s">
         <v>8</v>
@@ -3389,7 +3960,7 @@
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <f>Design!D83+2*Design!E83+4*Design!F83+8*Design!G83</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
@@ -3421,14 +3992,14 @@
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <f>Design!D85+2*Design!E85+4*Design!F85+8*Design!G85</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
       </c>
       <c r="C85">
         <f>Design!H85+2*Design!I85</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D85" t="s">
         <v>8</v>
@@ -3440,14 +4011,14 @@
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <f>Design!D86+2*Design!E86+4*Design!F86+8*Design!G86</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
       </c>
       <c r="C86">
         <f>Design!H86+2*Design!I86</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D86" t="s">
         <v>8</v>
@@ -3456,14 +4027,14 @@
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <f>Design!D87+2*Design!E87+4*Design!F87+8*Design!G87</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
       </c>
       <c r="C87">
         <f>Design!H87+2*Design!I87</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D87" t="s">
         <v>8</v>
@@ -3472,14 +4043,14 @@
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <f>Design!D88+2*Design!E88+4*Design!F88+8*Design!G88</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
       </c>
       <c r="C88">
         <f>Design!H88+2*Design!I88</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D88" t="s">
         <v>8</v>
@@ -3488,7 +4059,7 @@
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <f>Design!D89+2*Design!E89+4*Design!F89+8*Design!G89</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
@@ -3504,14 +4075,14 @@
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <f>Design!D90+2*Design!E90+4*Design!F90+8*Design!G90</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
       </c>
       <c r="C90">
         <f>Design!H90+2*Design!I90</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D90" t="s">
         <v>8</v>
@@ -3520,7 +4091,7 @@
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <f>Design!D91+2*Design!E91+4*Design!F91+8*Design!G91</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
@@ -3536,14 +4107,14 @@
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <f>Design!D92+2*Design!E92+4*Design!F92+8*Design!G92</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
       </c>
       <c r="C92">
         <f>Design!H92+2*Design!I92</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D92" t="s">
         <v>8</v>
@@ -3552,7 +4123,7 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <f>Design!D93+2*Design!E93+4*Design!F93+8*Design!G93</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B93" t="s">
         <v>8</v>
@@ -3584,14 +4155,14 @@
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <f>Design!D95+2*Design!E95+4*Design!F95+8*Design!G95</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B95" t="s">
         <v>8</v>
       </c>
       <c r="C95">
         <f>Design!H95+2*Design!I95</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D95" t="s">
         <v>8</v>
@@ -3603,14 +4174,14 @@
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <f>Design!D96+2*Design!E96+4*Design!F96+8*Design!G96</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B96" t="s">
         <v>8</v>
       </c>
       <c r="C96">
         <f>Design!H96+2*Design!I96</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D96" t="s">
         <v>8</v>
@@ -3619,14 +4190,14 @@
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <f>Design!D97+2*Design!E97+4*Design!F97+8*Design!G97</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B97" t="s">
         <v>8</v>
       </c>
       <c r="C97">
         <f>Design!H97+2*Design!I97</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D97" t="s">
         <v>8</v>
@@ -3635,14 +4206,14 @@
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <f>Design!D98+2*Design!E98+4*Design!F98+8*Design!G98</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
       </c>
       <c r="C98">
         <f>Design!H98+2*Design!I98</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98" t="s">
         <v>8</v>
@@ -3651,14 +4222,14 @@
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <f>Design!D99+2*Design!E99+4*Design!F99+8*Design!G99</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
       </c>
       <c r="C99">
         <f>Design!H99+2*Design!I99</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
         <v>8</v>
@@ -3667,14 +4238,14 @@
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <f>Design!D100+2*Design!E100+4*Design!F100+8*Design!G100</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
       </c>
       <c r="C100">
         <f>Design!H100+2*Design!I100</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D100" t="s">
         <v>8</v>
@@ -3683,7 +4254,7 @@
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <f>Design!D101+2*Design!E101+4*Design!F101+8*Design!G101</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B101" t="s">
         <v>8</v>
@@ -3699,14 +4270,14 @@
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <f>Design!D102+2*Design!E102+4*Design!F102+8*Design!G102</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
       </c>
       <c r="C102">
         <f>Design!H102+2*Design!I102</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D102" t="s">
         <v>8</v>
@@ -3715,7 +4286,7 @@
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <f>Design!D103+2*Design!E103+4*Design!F103+8*Design!G103</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
@@ -3758,7 +4329,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>